<commit_message>
Preliminary results for genetic, cars, myocardial and cirrhosis ok.
</commit_message>
<xml_diff>
--- a/Cars/rulex_results/Scoring_Rules_Cars_multi.xlsx
+++ b/Cars/rulex_results/Scoring_Rules_Cars_multi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/lucas_rizzo_tudublin_ie/Documents/rulex/Multiclass/Cars/rulex_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1D328510-0994-4934-BAC4-C14350432AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5BFB3A7-543E-4BCE-89C2-FC9617F556DE}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1D328510-0994-4934-BAC4-C14350432AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2989136-01AF-4890-999F-A122144F9671}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Max 0.050 Fold 1" sheetId="1" r:id="rId1"/>
@@ -560,18 +560,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -612,7 +614,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -653,7 +655,7 @@
         <v>0.257521</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -691,7 +693,7 @@
         <v>0.17078399999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -732,7 +734,7 @@
         <v>0.17078399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -773,7 +775,7 @@
         <v>0.12958800000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -811,7 +813,7 @@
         <v>9.4330999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -849,7 +851,7 @@
         <v>8.8496000000000005E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -887,7 +889,7 @@
         <v>8.8496000000000005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -928,7 +930,7 @@
         <v>0.66652900000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -966,7 +968,7 @@
         <v>0.33347100000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>0.242841</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1030,7 +1032,7 @@
         <v>0.242841</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>0.112396</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1109,7 +1111,7 @@
         <v>9.5656000000000005E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>9.1064999999999993E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1179,7 +1181,7 @@
         <v>9.1064999999999993E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>7.0808999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1252,7 +1254,7 @@
         <v>5.3326999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1305,18 +1307,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1357,7 +1361,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1395,7 +1399,7 @@
         <v>0.36596099999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1433,7 +1437,7 @@
         <v>0.31183499999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1471,7 +1475,7 @@
         <v>0.19264400000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1506,7 +1510,7 @@
         <v>0.12956000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1547,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>0.27135799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>0.27135799999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1646,7 +1650,7 @@
         <v>0.173593</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1681,7 +1685,7 @@
         <v>0.153308</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1719,7 +1723,7 @@
         <v>7.3084999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1754,7 +1758,7 @@
         <v>5.7297000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1804,18 +1808,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>0.51870499999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1926,7 +1932,7 @@
         <v>0.39054299999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1961,7 +1967,7 @@
         <v>9.0751999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>0.26828000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>0.26828000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>0.171624</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>0.15156800000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2168,7 +2174,7 @@
         <v>9.7627000000000005E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>4.2619999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2250,18 +2256,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2299,7 +2307,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2334,7 +2342,7 @@
         <v>0.536435</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2369,7 +2377,7 @@
         <v>0.463565</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2407,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2439,7 +2447,7 @@
         <v>0.26828000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2471,7 +2479,7 @@
         <v>0.26828000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2506,7 +2514,7 @@
         <v>0.171624</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2541,7 +2549,7 @@
         <v>0.15156800000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v>9.7627000000000005E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2611,7 +2619,7 @@
         <v>4.2619999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2655,6 +2663,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="35e04e53-8035-4693-a7c1-f4caf4429e95" xsi:nil="true"/>
@@ -2663,15 +2680,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2924,20 +2932,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24EB71DE-73C4-4338-9BE9-53700FCF5848}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A528B788-8EB5-45B0-8386-EBD61C48E48A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="35e04e53-8035-4693-a7c1-f4caf4429e95"/>
     <ds:schemaRef ds:uri="94dc1244-2250-4226-8a6d-024056f3e2cb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24EB71DE-73C4-4338-9BE9-53700FCF5848}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>